<commit_message>
ajout de données dans le set de données
</commit_message>
<xml_diff>
--- a/Database/jeu de données database.xlsx
+++ b/Database/jeu de données database.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\Desktop\Travail\PETUT S3\PETUT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Flo\Desktop\Travail\PETUT S3\PETUT\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12624" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12624" tabRatio="975" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
   <si>
     <t>id_Commentaire</t>
   </si>
@@ -128,6 +128,36 @@
   </si>
   <si>
     <t>Type_Utilisateur</t>
+  </si>
+  <si>
+    <t>IUT Informatique</t>
+  </si>
+  <si>
+    <t>133 Avenue de Rangueil, 31100 Toulouse</t>
+  </si>
+  <si>
+    <t>Bremec</t>
+  </si>
+  <si>
+    <t>Florian</t>
+  </si>
+  <si>
+    <t>17C Avenue du Gers, 31270 Frouzins</t>
+  </si>
+  <si>
+    <t>fbremec@gmail.com</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Magnaud</t>
+  </si>
+  <si>
+    <t>Patrick</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -151,7 +181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,6 +200,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7CC576"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -183,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
@@ -192,6 +228,12 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,9 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -721,21 +761,21 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -763,6 +803,165 @@
       </c>
       <c r="H1" s="3" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4">
+        <v>781734740</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" deleteRows="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="WorksheetGuid" r:id="rId1"/>
+  </customProperties>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" deleteRows="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <customProperties>
+    <customPr name="WorksheetGuid" r:id="rId2"/>
+  </customProperties>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -784,127 +983,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" deleteRows="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <customProperties>
-    <customPr name="WorksheetGuid" r:id="rId2"/>
-  </customProperties>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="I12:J12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" deleteRows="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="WorksheetGuid" r:id="rId1"/>
-  </customProperties>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
@@ -945,15 +1023,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -968,9 +1048,20 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" deleteRows="0"/>

</xml_diff>